<commit_message>
(feat) added create_documents to main and made mypy more strict.
</commit_message>
<xml_diff>
--- a/tests/templates/dummy_excel.xlsx
+++ b/tests/templates/dummy_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Projects\DocuCraft\tests\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A36150A-8FCD-458A-A428-11469E356E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57AC8CF-70A2-4646-853A-4BC4C39A9CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{E55224E5-BFEC-4CBA-974D-A4BE29760E17}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
   <si>
     <t>Address</t>
   </si>
@@ -154,8 +154,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77E22BF7-B975-45A9-8E9F-BE4F2EE1CE2F}" name="dummy_data" displayName="dummy_data" ref="A1:C62" totalsRowShown="0">
-  <autoFilter ref="A1:C62" xr:uid="{77E22BF7-B975-45A9-8E9F-BE4F2EE1CE2F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77E22BF7-B975-45A9-8E9F-BE4F2EE1CE2F}" name="dummy_data" displayName="dummy_data" ref="A1:C38" totalsRowShown="0">
+  <autoFilter ref="A1:C38" xr:uid="{77E22BF7-B975-45A9-8E9F-BE4F2EE1CE2F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{12F42FD2-6B22-4F65-843E-A0AF49369D03}" name="Address"/>
     <tableColumn id="2" xr3:uid="{1FFCF6D1-AA4A-4BB0-A511-3C224C9A1850}" name="Item"/>
@@ -482,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27910B1-97A6-4387-9355-FEF543E8D48D}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +533,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>492.82</v>
+        <v>990.33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,32 +544,32 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>282.54000000000002</v>
+        <v>983.65</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>990.33</v>
+        <v>105.84</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>983.65</v>
+        <v>686.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -577,10 +577,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
-        <v>105.84</v>
+        <v>434.85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,10 +588,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>686.6</v>
+        <v>634.16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -599,65 +599,65 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>988.58</v>
+        <v>773.19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>434.85</v>
+        <v>444.25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>634.16</v>
+        <v>98.39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>773.19</v>
+        <v>71.64</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1">
-        <v>444.25</v>
+        <v>129.41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1">
-        <v>98.39</v>
+        <v>420.1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,10 +665,10 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1">
-        <v>71.64</v>
+        <v>132.88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,504 +676,240 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>129.41</v>
+        <v>344.53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="1">
-        <v>420.1</v>
+        <v>711.38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
-        <v>16.23</v>
+        <v>184.24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1">
-        <v>575.07000000000005</v>
+        <v>621.98</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1">
-        <v>999.76</v>
+        <v>548.14</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1">
-        <v>132.88</v>
+        <v>804.93</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1">
-        <v>344.53</v>
+        <v>892.47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1">
-        <v>63.89</v>
+        <v>719.05</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1">
-        <v>440.09</v>
+        <v>465.22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1">
-        <v>711.38</v>
+        <v>400.53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1">
-        <v>184.24</v>
+        <v>677.01</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="1">
-        <v>621.98</v>
+        <v>360.96</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1">
-        <v>680</v>
+        <v>156.53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C30" s="1">
-        <v>758.83</v>
+        <v>138.53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1">
-        <v>548.14</v>
+        <v>553.65</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1">
-        <v>550.91999999999996</v>
+        <v>929.13</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C33" s="1">
-        <v>782.06</v>
+        <v>93.58</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34" s="1">
-        <v>787.74</v>
+        <v>188.46</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1">
-        <v>208.4</v>
+        <v>873.02</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="1">
-        <v>804.93</v>
+        <v>523.78</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="1">
-        <v>432.48</v>
+        <v>341.67</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" s="1">
-        <v>48.86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="1">
-        <v>892.47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="1">
-        <v>719.05</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="1">
-        <v>584.01</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="1">
-        <v>465.22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="1">
-        <v>251.3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="1">
-        <v>896.75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="1">
-        <v>400.53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="1">
-        <v>632.07000000000005</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="1">
-        <v>677.01</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="1">
-        <v>692.37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="1">
-        <v>727.41</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="1">
-        <v>360.96</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="1">
-        <v>156.53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>15</v>
-      </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="1">
-        <v>138.53</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>15</v>
-      </c>
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" s="1">
-        <v>552.19000000000005</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>15</v>
-      </c>
-      <c r="B54" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" s="1">
-        <v>867.43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>15</v>
-      </c>
-      <c r="B55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="1">
-        <v>553.65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>15</v>
-      </c>
-      <c r="B56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="1">
-        <v>929.13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="1">
-        <v>93.58</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="1">
-        <v>188.46</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>16</v>
-      </c>
-      <c r="B59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="1">
-        <v>873.02</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>16</v>
-      </c>
-      <c r="B60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="1">
-        <v>523.78</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" s="1">
-        <v>341.67</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="1">
         <v>440.05</v>
       </c>
     </row>

</xml_diff>